<commit_message>
Was working on it during the classes and stored it in my X drive, now pushing the final project
Signed-off-by: Modestas Cepulis <Modestas.Cepulis@students.ittralee.ie>
</commit_message>
<xml_diff>
--- a/M.C. Assignment 1.xlsx
+++ b/M.C. Assignment 1.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t00199237\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\students\t00199237\YEAR 3\Graphics Design\assigmentus\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="62">
   <si>
     <t>z = -1</t>
   </si>
@@ -143,12 +143,149 @@
 -1,-1,-1
 1,-1,-1</t>
   </si>
+  <si>
+    <t>0.9877838 , 1.23291 , 0.7100809</t>
+  </si>
+  <si>
+    <t>-1.007905 , 1.150707 , 0.8124053</t>
+  </si>
+  <si>
+    <t>-0.9055802 , -0.8001891 , 1.240815</t>
+  </si>
+  <si>
+    <t>1.090108 , -0.7179855 , 1.138491</t>
+  </si>
+  <si>
+    <t>0.9055802 , 0.8001891 , -1.240815</t>
+  </si>
+  <si>
+    <t>-1.090108 , 0.7179855 , -1.138491</t>
+  </si>
+  <si>
+    <t>-0.9877838 , -1.23291 , -0.7100809</t>
+  </si>
+  <si>
+    <t>1.007905 , -1.150707 , -0.8124053</t>
+  </si>
+  <si>
+    <t>0.9978442 , -0.05116219 , 0.04110185
+0.04110185 , 0.975448 , 0.2163606
+-0.05116219 , -0.2142049 , 0.975448</t>
+  </si>
+  <si>
+    <t>14.82897 , 7.164552 , 3.130243
+-13.11066 , 6.753534 , 3.437216
+-11.67812 , -3.000946 , 4.722445
+16.26152 , -2.589927 , 4.415472
+13.67812 , 5.000946 , -2.722445
+-14.26152 , 4.589927 , -2.415472
+-12.82897 , -5.164552 , -1.130243
+15.11066 , -4.753534 , -1.437216</t>
+  </si>
+  <si>
+    <t>14 0 0 0
+0 5 0 0 
+0 0 3 0
+0 0 0 1</t>
+  </si>
+  <si>
+    <t>0 0 0 2
+0 0 0 -2
+0 0 0 -2
+0 0 0 1</t>
+  </si>
+  <si>
+    <t>15.82897 , 4.164552 , 0.1302428
+-12.11066 , 3.753534 , 0.4372158
+-10.67812 , -6.000946 , 1.722445
+17.26152 , -5.589927 , 1.415472
+14.67812 , 2.000946 , -5.722445
+-13.26152 , 1.589927 , -5.415472
+-11.82897 , -8.164552 , -4.130243
+16.11066 , -7.753534 , -4.437216</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-0.2, -0.9, -0.4, -16.0)
+(-1.0, 0.1, 0.3, 0.0)
+(-0.2, 0.4, -0.9, -47.0)
+(0.0, 0.0, 0.0, 1.0)
+</t>
+  </si>
+  <si>
+    <t>(-22.57332 , -14.85153 , -49.0348
+-17.47931 , 11.96495 , -43.05032
+-9.355297 , 10.31866 , -48.54068
+-14.44931 , -16.49782 , -54.52516
+-18.18147 , -15.53123 , -44.50609
+-13.08746 , 11.28525 , -38.5216
+-4.963447 , 9.638958 , -44.01196
+-10.05746 , -17.17752 , -49.99644)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1.5, 0.0, 0.0, 0.0)
+(0.0, 2.4, 0.0, 0.0)
+(0.0, 0.0, -1.0, -2.0)
+(0.0, 0.0, -1.0, 0.0)
+</t>
+  </si>
+  <si>
+    <t>(-34.06051 , -35.85476 , 47.15504
+-26.37424 , 28.88594 , 41.15558
+-14.11605 , 24.91144 , 46.65968
+-21.80232 , -39.82926 , 52.65915
+-27.43372 , -37.4957 , 42.61499
+-19.74745 , 27.245 , 36.61552
+-7.489262 , 23.2705 , 42.11963
+-15.17553 , -41.4702 , 48.11909)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-3.8, -6.1, -3.3, -20.8)
+(-32.4, 2.0, 0.8, -6.3)
+(3.0, -2.8, 2.3, 44.6)
+(3.0, -2.7, 2.3, 46.5)
+</t>
+  </si>
+  <si>
+    <t>(-34.0605 , -35.85476 , 47.15504
+-26.37424 , 28.88594 , 41.15558
+-14.11605 , 24.91144 , 46.65968
+-21.80232 , -39.82926 , 52.65915
+-27.43372 , -37.4957 , 42.61499
+-19.74744 , 27.245 , 36.61553
+-7.489261 , 23.2705 , 42.11963
+-15.17553 , -41.4702 , 48.11909)</t>
+  </si>
+  <si>
+    <t>(14.0, -0.7, 0.6, 2.0)
+(0.2, 4.9, 1.1, -2.0)
+(-0.2, -0.6, 2.9, -2.0)
+(0.0, 0.0, 0.0, 1.0)</t>
+  </si>
+  <si>
+    <t>(15.82897 , 4.164552 , 0.1302427
+-12.11066 , 3.753534 , 0.4372159
+-10.67812 , -6.000946 , 1.722445
+17.26152 , -5.589927 , 1.415472
+14.67812 , 2.000946 , -5.722445
+-13.26152 , 1.589927 , -5.415472
+-11.82897 , -8.164552 , -4.130243
+16.11066 , -7.753534 , -4.437216</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Projection By Hand</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -157,6 +294,12 @@
     <font>
       <sz val="10"/>
       <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -326,7 +469,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -408,6 +551,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -447,6 +593,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,6 +620,3847 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IE"/>
+              <a:t>Projection By Hand</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet3!$G$17:$G$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>-0.46035305538107629</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.40602044305361729</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.1927310659842425</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.26500261530640168</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.40851645246751628</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.33974341668051172</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.11277495935195797</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.20116352284282643</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet3!$H$17:$H$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>-0.30287734425346902</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27792940911937475</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.21257757410897415</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.30257261051595263</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.34896864676272393</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.29295901520186074</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.21900769699872488</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.34357486253021219</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6864-4EBC-AF8E-95EB49600808}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1400782208"/>
+        <c:axId val="1400782624"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1400782208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1400782624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1400782624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1400782208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IE"/>
+              <a:t>Final Image</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet3!$G$27:$G$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>-0.72230900450938018</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.64084238394890802</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.30253207908841206</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.41402719185554654</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.6437575134946647</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.5393191193242648</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.1778093017436288</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.31537441792851861</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.31537441792851861</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet3!$H$27:$H$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>-0.76035901994781463</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.70187177534613776</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.53389650336221761</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.75635972096017501</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.87987114393315591</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.74408338322110412</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5524858599185225</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.86182427805679618</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.86182427805679618</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8C50-499C-83AF-912D2164169F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1409470608"/>
+        <c:axId val="1409474352"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1409470608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1409474352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1409474352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1409470608"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IE"/>
+              <a:t>Projection By Hand</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet3!$G$17:$G$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>-0.46035305538107629</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.40602044305361729</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.1927310659842425</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.26500261530640168</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.40851645246751628</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.33974341668051172</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.11277495935195797</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.20116352284282643</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet3!$H$17:$H$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>-0.30287734425346902</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27792940911937475</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.21257757410897415</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.30257261051595263</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.34896864676272393</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.29295901520186074</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.21900769699872488</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.34357486253021219</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8786-4CFD-81EE-6F923593824D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1400782208"/>
+        <c:axId val="1400782624"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1400782208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1400782624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1400782624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1400782208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IE"/>
+              <a:t>Final Image</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet3!$G$27:$G$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>-0.72230900450938018</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.64084238394890802</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.30253207908841206</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.41402719185554654</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.6437575134946647</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.5393191193242648</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.1778093017436288</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.31537441792851861</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.31537441792851861</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet3!$H$27:$H$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>-0.76035901994781463</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.70187177534613776</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.53389650336221761</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.75635972096017501</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.87987114393315591</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.74408338322110412</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5524858599185225</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.86182427805679618</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.86182427805679618</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-839B-478D-9878-E0305311636E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1409470608"/>
+        <c:axId val="1409474352"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1409470608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1409474352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1409474352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1409470608"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1265989</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1524000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1943100" y="3352800"/>
+          <a:ext cx="3656764" cy="1524000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1228725</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -753,8 +4752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -766,24 +4765,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
     </row>
     <row r="2" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
     </row>
     <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -951,8 +4950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -976,10 +4975,10 @@
     </row>
     <row r="2" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C2" s="5"/>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="30"/>
+      <c r="E2" s="31"/>
       <c r="F2" s="8"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -990,10 +4989,10 @@
     </row>
     <row r="3" spans="3:13" ht="111" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="5"/>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="32"/>
+      <c r="E3" s="33"/>
       <c r="F3" s="6"/>
       <c r="G3" s="11"/>
       <c r="H3" s="7"/>
@@ -1013,10 +5012,10 @@
     </row>
     <row r="5" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="5"/>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="30"/>
+      <c r="E5" s="31"/>
       <c r="F5" s="8"/>
       <c r="H5" s="15"/>
       <c r="I5" s="12"/>
@@ -1025,8 +5024,10 @@
     </row>
     <row r="6" spans="3:13" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="5"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="32"/>
+      <c r="D6" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="33"/>
       <c r="F6" s="16"/>
       <c r="G6" s="12"/>
       <c r="H6" s="15"/>
@@ -1046,10 +5047,10 @@
     </row>
     <row r="8" spans="3:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="5"/>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="30"/>
+      <c r="E8" s="31"/>
       <c r="F8" s="17"/>
       <c r="G8" s="12"/>
       <c r="H8" s="15"/>
@@ -1059,11 +5060,11 @@
     </row>
     <row r="9" spans="3:13" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="5"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="32"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="40"/>
       <c r="F9" s="17"/>
       <c r="G9" s="12"/>
-      <c r="H9" s="15"/>
+      <c r="H9" s="27"/>
       <c r="I9" s="12"/>
       <c r="L9" s="15"/>
       <c r="M9" s="12"/>
@@ -1080,28 +5081,32 @@
     </row>
     <row r="11" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="5"/>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="30"/>
+      <c r="E11" s="31"/>
       <c r="F11" s="18"/>
       <c r="G11" s="19"/>
-      <c r="H11" s="37" t="s">
+      <c r="H11" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="38"/>
+      <c r="I11" s="39"/>
       <c r="J11" s="8"/>
       <c r="L11" s="15"/>
       <c r="M11" s="12"/>
     </row>
     <row r="12" spans="3:13" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="5"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="39"/>
+      <c r="D12" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="40"/>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="39"/>
+      <c r="H12" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="I12" s="40"/>
       <c r="J12" s="16"/>
       <c r="K12" s="12"/>
       <c r="L12" s="15"/>
@@ -1121,10 +5126,10 @@
     </row>
     <row r="14" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C14" s="5"/>
-      <c r="D14" s="29" t="s">
+      <c r="D14" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="30"/>
+      <c r="E14" s="31"/>
       <c r="F14" s="17"/>
       <c r="G14" s="12"/>
       <c r="H14" s="15"/>
@@ -1136,8 +5141,10 @@
     </row>
     <row r="15" spans="3:13" ht="121.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C15" s="5"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="32"/>
+      <c r="D15" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="40"/>
       <c r="F15" s="17"/>
       <c r="G15" s="12"/>
       <c r="H15" s="15"/>
@@ -1161,10 +5168,10 @@
     </row>
     <row r="17" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C17" s="5"/>
-      <c r="D17" s="29" t="s">
+      <c r="D17" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="30"/>
+      <c r="E17" s="31"/>
       <c r="F17" s="18"/>
       <c r="G17" s="12"/>
       <c r="H17" s="15"/>
@@ -1176,8 +5183,10 @@
     </row>
     <row r="18" spans="1:13" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C18" s="5"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="39"/>
+      <c r="D18" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="40"/>
       <c r="F18" s="20"/>
       <c r="H18" s="15"/>
       <c r="I18" s="12"/>
@@ -1198,18 +5207,18 @@
     </row>
     <row r="20" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C20" s="5"/>
-      <c r="D20" s="29" t="s">
+      <c r="D20" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="30"/>
-      <c r="F20" s="34" t="s">
+      <c r="E20" s="31"/>
+      <c r="F20" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="36"/>
-      <c r="H20" s="37" t="s">
+      <c r="G20" s="37"/>
+      <c r="H20" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="I20" s="38"/>
+      <c r="I20" s="39"/>
       <c r="J20" s="17"/>
       <c r="K20" s="12"/>
       <c r="L20" s="15"/>
@@ -1217,12 +5226,16 @@
     </row>
     <row r="21" spans="1:13" ht="114" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C21" s="5"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="39"/>
+      <c r="D21" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="33"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="I21" s="40"/>
       <c r="J21" s="17"/>
       <c r="K21" s="12"/>
       <c r="L21" s="15"/>
@@ -1240,33 +5253,37 @@
     </row>
     <row r="23" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C23" s="5"/>
-      <c r="D23" s="29" t="s">
+      <c r="D23" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="30"/>
+      <c r="E23" s="31"/>
       <c r="F23" s="9"/>
       <c r="G23" s="22"/>
       <c r="H23" s="22"/>
       <c r="I23" s="22"/>
       <c r="J23" s="10"/>
       <c r="K23" s="18"/>
-      <c r="L23" s="37" t="s">
+      <c r="L23" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="M23" s="38"/>
+      <c r="M23" s="39"/>
     </row>
     <row r="24" spans="1:13" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C24" s="5"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="39"/>
+      <c r="D24" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" s="40"/>
       <c r="F24" s="6"/>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
       <c r="J24" s="7"/>
       <c r="K24" s="23"/>
-      <c r="L24" s="33"/>
-      <c r="M24" s="39"/>
+      <c r="L24" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="M24" s="40"/>
     </row>
     <row r="25" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D25" s="13"/>
@@ -1279,10 +5296,10 @@
     <row r="26" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="4"/>
       <c r="C26" s="24"/>
-      <c r="D26" s="37" t="s">
+      <c r="D26" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="38"/>
+      <c r="E26" s="39"/>
       <c r="F26" s="12"/>
       <c r="J26" s="15"/>
       <c r="K26" s="12"/>
@@ -1293,8 +5310,10 @@
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="39"/>
+      <c r="D27" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27" s="40"/>
       <c r="F27" s="12"/>
       <c r="J27" s="15"/>
       <c r="K27" s="12"/>
@@ -1312,15 +5331,15 @@
       <c r="M28" s="12"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="38"/>
+      <c r="B29" s="39"/>
       <c r="C29" s="25"/>
-      <c r="D29" s="29" t="s">
+      <c r="D29" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="E29" s="30"/>
+      <c r="E29" s="31"/>
       <c r="F29" s="9"/>
       <c r="G29" s="22"/>
       <c r="H29" s="22"/>
@@ -1331,11 +5350,13 @@
       <c r="M29" s="12"/>
     </row>
     <row r="30" spans="1:13" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="33"/>
-      <c r="B30" s="39"/>
+      <c r="A30" s="34"/>
+      <c r="B30" s="40"/>
       <c r="C30" s="25"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="39"/>
+      <c r="D30" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="E30" s="40"/>
       <c r="F30" s="20"/>
       <c r="G30" s="21"/>
       <c r="H30" s="21"/>
@@ -1353,44 +5374,48 @@
       <c r="M31" s="8"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="29" t="s">
+      <c r="A32" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="30"/>
+      <c r="B32" s="31"/>
       <c r="C32" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="29" t="s">
+      <c r="D32" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="E32" s="30"/>
-      <c r="F32" s="34" t="s">
+      <c r="E32" s="31"/>
+      <c r="F32" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="G32" s="35"/>
-      <c r="H32" s="35"/>
-      <c r="I32" s="35"/>
-      <c r="J32" s="35"/>
-      <c r="K32" s="36"/>
-      <c r="L32" s="29" t="s">
+      <c r="G32" s="36"/>
+      <c r="H32" s="36"/>
+      <c r="I32" s="36"/>
+      <c r="J32" s="36"/>
+      <c r="K32" s="37"/>
+      <c r="L32" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="M32" s="30"/>
+      <c r="M32" s="31"/>
     </row>
     <row r="33" spans="1:13" ht="116.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="31"/>
-      <c r="B33" s="32"/>
+      <c r="A33" s="32"/>
+      <c r="B33" s="33"/>
       <c r="C33" s="17"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="35"/>
-      <c r="H33" s="35"/>
-      <c r="I33" s="35"/>
-      <c r="J33" s="35"/>
-      <c r="K33" s="36"/>
-      <c r="L33" s="33"/>
-      <c r="M33" s="32"/>
+      <c r="D33" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="E33" s="33"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="36"/>
+      <c r="H33" s="36"/>
+      <c r="I33" s="36"/>
+      <c r="J33" s="36"/>
+      <c r="K33" s="37"/>
+      <c r="L33" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="M33" s="33"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="21"/>
@@ -1402,23 +5427,23 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C35" s="5"/>
-      <c r="D35" s="37" t="s">
+      <c r="D35" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="E35" s="38"/>
+      <c r="E35" s="39"/>
       <c r="F35" s="12"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C36" s="5"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="39"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="40"/>
       <c r="F36" s="12"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E38" s="26"/>
       <c r="F38" s="26"/>
-      <c r="H38" s="33"/>
-      <c r="I38" s="32"/>
+      <c r="H38" s="34"/>
+      <c r="I38" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="41">
@@ -1467,22 +5492,415 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:N35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:H35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="6" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="48.28515625" customWidth="1"/>
+    <col min="2" max="6" width="9.140625" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" t="s">
+        <v>59</v>
+      </c>
+      <c r="H16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C17" s="43">
+        <v>-22.573319999999999</v>
+      </c>
+      <c r="D17" s="44">
+        <v>-14.85153</v>
+      </c>
+      <c r="E17" s="44">
+        <v>-49.034799999999997</v>
+      </c>
+      <c r="G17">
+        <f>C17/-E17</f>
+        <v>-0.46035305538107629</v>
+      </c>
+      <c r="H17">
+        <f>D17/-E17</f>
+        <v>-0.30287734425346902</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <v>-17.479310000000002</v>
+      </c>
+      <c r="D18">
+        <v>11.96495</v>
+      </c>
+      <c r="E18">
+        <v>-43.050319999999999</v>
+      </c>
+      <c r="G18">
+        <f t="shared" ref="G18:G24" si="0">C18/-E18</f>
+        <v>-0.40602044305361729</v>
+      </c>
+      <c r="H18">
+        <f t="shared" ref="H18:H24" si="1">D18/-E18</f>
+        <v>0.27792940911937475</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C19">
+        <v>-9.3552970000000002</v>
+      </c>
+      <c r="D19">
+        <v>10.318659999999999</v>
+      </c>
+      <c r="E19">
+        <v>-48.540680000000002</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>-0.1927310659842425</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>0.21257757410897415</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C20">
+        <v>-14.449310000000001</v>
+      </c>
+      <c r="D20">
+        <v>-16.497820000000001</v>
+      </c>
+      <c r="E20">
+        <v>-54.52516</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>-0.26500261530640168</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="1"/>
+        <v>-0.30257261051595263</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C21">
+        <v>-18.181470000000001</v>
+      </c>
+      <c r="D21">
+        <v>-15.531230000000001</v>
+      </c>
+      <c r="E21">
+        <v>-44.50609</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>-0.40851645246751628</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="1"/>
+        <v>-0.34896864676272393</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C22">
+        <v>-13.08746</v>
+      </c>
+      <c r="D22">
+        <v>11.28525</v>
+      </c>
+      <c r="E22">
+        <v>-38.521599999999999</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>-0.33974341668051172</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="1"/>
+        <v>0.29295901520186074</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C23">
+        <v>-4.9634470000000004</v>
+      </c>
+      <c r="D23">
+        <v>9.6389580000000006</v>
+      </c>
+      <c r="E23">
+        <v>-44.011960000000002</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>-0.11277495935195797</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="1"/>
+        <v>0.21900769699872488</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C24">
+        <v>-10.057460000000001</v>
+      </c>
+      <c r="D24">
+        <v>-17.177520000000001</v>
+      </c>
+      <c r="E24">
+        <v>-49.99644</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>-0.20116352284282643</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="1"/>
+        <v>-0.34357486253021219</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C27" s="42">
+        <v>-34.060510000000001</v>
+      </c>
+      <c r="D27">
+        <v>-35.854759999999999</v>
+      </c>
+      <c r="E27">
+        <v>47.15504</v>
+      </c>
+      <c r="G27">
+        <f>C27/E27</f>
+        <v>-0.72230900450938018</v>
+      </c>
+      <c r="H27">
+        <f>D27/E27</f>
+        <v>-0.76035901994781463</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C28" s="41">
+        <v>-26.37424</v>
+      </c>
+      <c r="D28">
+        <v>28.885940000000002</v>
+      </c>
+      <c r="E28">
+        <v>41.15558</v>
+      </c>
+      <c r="G28">
+        <f t="shared" ref="G28:G35" si="2">C28/E28</f>
+        <v>-0.64084238394890802</v>
+      </c>
+      <c r="H28">
+        <f t="shared" ref="H28:H35" si="3">D28/E28</f>
+        <v>0.70187177534613776</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C29">
+        <v>-14.11605</v>
+      </c>
+      <c r="D29">
+        <v>24.911439999999999</v>
+      </c>
+      <c r="E29">
+        <v>46.659680000000002</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="2"/>
+        <v>-0.30253207908841206</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="3"/>
+        <v>0.53389650336221761</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C30">
+        <v>-21.802320000000002</v>
+      </c>
+      <c r="D30">
+        <v>-39.829259999999998</v>
+      </c>
+      <c r="E30">
+        <v>52.659149999999997</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="2"/>
+        <v>-0.41402719185554654</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="3"/>
+        <v>-0.75635972096017501</v>
+      </c>
+      <c r="M30" s="34"/>
+      <c r="N30" s="33"/>
+    </row>
+    <row r="31" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C31">
+        <v>-27.433720000000001</v>
+      </c>
+      <c r="D31">
+        <v>-37.495699999999999</v>
+      </c>
+      <c r="E31">
+        <v>42.614989999999999</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="2"/>
+        <v>-0.6437575134946647</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="3"/>
+        <v>-0.87987114393315591</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C32">
+        <v>-19.747450000000001</v>
+      </c>
+      <c r="D32">
+        <v>27.245000000000001</v>
+      </c>
+      <c r="E32">
+        <v>36.615519999999997</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="2"/>
+        <v>-0.5393191193242648</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="3"/>
+        <v>0.74408338322110412</v>
+      </c>
+    </row>
+    <row r="33" spans="3:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C33">
+        <v>-7.4892620000000001</v>
+      </c>
+      <c r="D33">
+        <v>23.270499999999998</v>
+      </c>
+      <c r="E33">
+        <v>42.119630000000001</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="2"/>
+        <v>-0.1778093017436288</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="3"/>
+        <v>0.5524858599185225</v>
+      </c>
+    </row>
+    <row r="34" spans="3:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C34">
+        <v>-15.17553</v>
+      </c>
+      <c r="D34">
+        <v>-41.470199999999998</v>
+      </c>
+      <c r="E34">
+        <v>48.11909</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="2"/>
+        <v>-0.31537441792851861</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="3"/>
+        <v>-0.86182427805679618</v>
+      </c>
+    </row>
+    <row r="35" spans="3:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C35">
+        <v>-15.17553</v>
+      </c>
+      <c r="D35">
+        <v>-41.470199999999998</v>
+      </c>
+      <c r="E35">
+        <v>48.11909</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="2"/>
+        <v>-0.31537441792851861</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="3"/>
+        <v>-0.86182427805679618</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="M30:N30"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>